<commit_message>
Added normalization loss image
</commit_message>
<xml_diff>
--- a/data/normalization.xlsx
+++ b/data/normalization.xlsx
@@ -1198,7 +1198,1140 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="2000"/>
+              <a:t>objective</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12704731660400184"/>
+          <c:y val="0.12072640361295618"/>
+          <c:w val="0.8405329366126304"/>
+          <c:h val="0.61957066819161566"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$X$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>without nor-layer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$W$3:$W$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>49</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$X$3:$X$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>2.5114083700000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.6369408999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0800106E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9041894000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3339376000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0081669000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.7861399999999996E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.4117590000000004E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.3746920000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.8965499999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.6181480000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.209401E-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.3222719999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.769046E-4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.416723E-4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.2688150000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.4739200000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.3062229999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.1585320000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.0807749999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.6793250000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.1328810000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.5005140000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.3763199999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.1474440000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.078294E-4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.1559200000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.0325090000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.0035149999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.9801630000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.9619470000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.9445280000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.9261389999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.907532E-4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.8923810000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.8748750000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.8612389999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.8452719999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.828347E-4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.8143919999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2.7990250000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2.7858469999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2.7714439999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2.7578489999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.7444060000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2.7310499999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2.7190820000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.7030510000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.691344E-4</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.6797270000000002E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4DBE-4F1D-B7DE-FCA8EED51C6B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Y$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>with nor-layer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$W$3:$W$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>49</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Y$3:$Y$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>2.4316685300000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.5685264E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.9511361000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9091734E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2172785E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.916563E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.4505830000000004E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.4438039999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0184989999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.7704429999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.2467280000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.0271159999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.6879490000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.6166710000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.6410290000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.3732130000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.8157689999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.420354E-4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.4508180000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.3722450000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.223352E-4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.0750869999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.0061390000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.9735420000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.9460169999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.9252219999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.9053450000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.8886420000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.872506E-4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.8520979999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.8379860000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.8210790000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.8060010000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.7878510000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.771742E-4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.7599249999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.7445969999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.7299490000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.7157610000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.7025699999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.1646430000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3.0345589999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2.870029E-4</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2.8165010000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.7573810000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2.7260320000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2.706494E-4</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.6916579999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.6741790000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.6586859999999998E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4DBE-4F1D-B7DE-FCA8EED51C6B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="438521056"/>
+        <c:axId val="438520072"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="438521056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1800"/>
+                  <a:t>training epoch</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="b" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="438520072"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="438520072"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1800"/>
+                  <a:t>loss</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="438521056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1754,6 +2887,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1787,6 +3436,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>485774</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F210AD20-F731-4A49-9F8D-951D9B636837}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2094,8 +3779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2FA4E76-D5F0-4671-9E99-BA51B0620FAC}">
   <dimension ref="B1:Y52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X31" workbookViewId="0">
-      <selection activeCell="AH52" sqref="AH52"/>
+    <sheetView tabSelected="1" topLeftCell="AH31" workbookViewId="0">
+      <selection activeCell="AV45" sqref="AV45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>